<commit_message>
commit 06-02-2018 at 6:29 PM
</commit_message>
<xml_diff>
--- a/RESTAutomation/src/main/java/com/api/config/API_Datapool.xlsx
+++ b/RESTAutomation/src/main/java/com/api/config/API_Datapool.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14145" windowHeight="3000"/>
   </bookViews>
   <sheets>
     <sheet name="Script1" sheetId="1" r:id="rId1"/>
     <sheet name="Script2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:M8"/>
 </workbook>
 </file>
 
@@ -400,7 +401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -459,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
commit at 06-02-2018 at 7:40 PM
</commit_message>
<xml_diff>
--- a/RESTAutomation/src/main/java/com/api/config/API_Datapool.xlsx
+++ b/RESTAutomation/src/main/java/com/api/config/API_Datapool.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14145" windowHeight="3000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14145" windowHeight="2445"/>
   </bookViews>
   <sheets>
     <sheet name="Script1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>TCName</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>/api/{users}/</t>
+  </si>
+  <si>
+    <t>/api/users/{user}</t>
   </si>
 </sst>
 </file>
@@ -407,7 +410,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -443,7 +446,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="3">

</xml_diff>